<commit_message>
Add view project_base and export excel in pabi_drilldown
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_unit_base_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_unit_base_report.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">Budget Section Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Type</t>
   </si>
   <si>
     <t xml:space="preserve">Fiscal Year</t>
@@ -317,10 +320,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,7 +412,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -418,57 +421,62 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" s="8" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="20" s="8" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="I20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="J20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="K20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="7" t="s">
+      <c r="M20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="N20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P19" s="7" t="s">
+      <c r="O20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q19" s="7" t="s">
+      <c r="P20" s="7" t="s">
         <v>29</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>